<commit_message>
Decoupling caps & more
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37646DF2-23A7-4AF8-A9D0-AFF04B651ED6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED586E5A-274E-4DEC-B5DE-C26E884ED630}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>HDC2010YPAR</t>
   </si>
   <si>
-    <t>PIC32MX795F512L-80I/PT</t>
-  </si>
-  <si>
     <t>LIS3DHTR</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>Accelerometer</t>
   </si>
   <si>
-    <t>CAM-M8C</t>
-  </si>
-  <si>
-    <t>U-Blox</t>
-  </si>
-  <si>
     <t>TC1014-5.0VCT713</t>
   </si>
   <si>
@@ -399,6 +390,15 @@
   </si>
   <si>
     <t>Nexperia</t>
+  </si>
+  <si>
+    <t>PIC32MX795F512L-80I/BG</t>
+  </si>
+  <si>
+    <t>MAX2771ETI+</t>
+  </si>
+  <si>
+    <t>Maxim</t>
   </si>
 </sst>
 </file>
@@ -650,6 +650,15 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,15 +666,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -957,7 +957,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +970,7 @@
     <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="38" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="35" customWidth="1"/>
     <col min="10" max="10" width="62.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" style="26" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -989,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1001,30 +1001,30 @@
         <v>4</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1033,27 +1033,27 @@
         <v>6</v>
       </c>
       <c r="D2" s="8">
-        <v>9.69</v>
+        <v>10.08</v>
       </c>
       <c r="E2" s="8">
-        <v>8.0442999999999998</v>
+        <v>8.3739000000000008</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="8">
         <f t="shared" ref="G2:G24" si="0">F2*E2</f>
-        <v>8.0442999999999998</v>
+        <v>8.3739000000000008</v>
       </c>
       <c r="H2" s="13">
         <f t="shared" ref="H2:H11" si="1">G2/$G$26</f>
-        <v>9.649405223439457E-2</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>122</v>
+        <v>0.10865689443624385</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>119</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="14">
@@ -1063,18 +1063,18 @@
         <v>98.69</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="8">
         <v>1.66</v>
@@ -1091,13 +1091,13 @@
       </c>
       <c r="H3" s="13">
         <f t="shared" si="1"/>
-        <v>1.8472811859449257E-2</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>121</v>
+        <v>1.9982519188408689E-2</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K3" s="24"/>
       <c r="L3" s="14">
@@ -1107,18 +1107,18 @@
         <v>80.599999999999994</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="8">
         <v>0.79</v>
@@ -1135,57 +1135,57 @@
       </c>
       <c r="H4" s="13">
         <f t="shared" si="1"/>
-        <v>8.5070897212476699E-3</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>121</v>
+        <v>9.2023393561165203E-3</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="D5" s="8">
-        <v>31.43</v>
+        <v>7.36</v>
       </c>
       <c r="E5" s="8">
-        <v>12</v>
+        <v>5.4720000000000004</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>5.4720000000000004</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>0.143943988515189</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>121</v>
+        <v>7.1002821427904123E-2</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1205,17 +1205,17 @@
       </c>
       <c r="H6" s="13">
         <f t="shared" si="1"/>
-        <v>3.0887980868884307E-3</v>
-      </c>
-      <c r="I6" s="36"/>
+        <v>3.3412329162436603E-3</v>
+      </c>
+      <c r="I6" s="33"/>
       <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -1235,22 +1235,22 @@
       </c>
       <c r="H7" s="13">
         <f t="shared" si="1"/>
-        <v>4.2511457941485815E-3</v>
-      </c>
-      <c r="I7" s="36" t="s">
-        <v>121</v>
+        <v>4.5985745456961291E-3</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="8">
         <v>43</v>
@@ -1267,22 +1267,22 @@
       </c>
       <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>0.40748383988822279</v>
-      </c>
-      <c r="I8" s="36" t="s">
-        <v>121</v>
+        <v>0.4407858268403122</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -1302,20 +1302,20 @@
       </c>
       <c r="H9" s="13">
         <f t="shared" si="1"/>
-        <v>7.005394061062961E-3</v>
-      </c>
-      <c r="I9" s="36"/>
+        <v>7.5779162540406224E-3</v>
+      </c>
+      <c r="I9" s="33"/>
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" s="6">
         <v>5.71</v>
@@ -1332,20 +1332,20 @@
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>4.2535448606238348E-2</v>
-      </c>
-      <c r="I10" s="36"/>
+        <v>4.6011696780582596E-2</v>
+      </c>
+      <c r="I10" s="33"/>
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="8">
         <v>3.58</v>
@@ -1362,22 +1362,22 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="1"/>
-        <v>3.3895210695614131E-2</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>121</v>
+        <v>3.666532757836781E-2</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" s="8">
         <v>0.47</v>
@@ -1393,20 +1393,20 @@
         <v>0.31950000000000001</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="36" t="s">
-        <v>121</v>
+      <c r="I12" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" s="8">
         <v>0.77</v>
@@ -1423,25 +1423,25 @@
       </c>
       <c r="H13" s="13">
         <f t="shared" ref="H13:H24" si="2">G13/$G$26</f>
-        <v>7.3118748032765506E-3</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>121</v>
+        <v>7.9094444133028571E-3</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="8">
         <v>2.6</v>
@@ -1458,25 +1458,25 @@
       </c>
       <c r="H14" s="13">
         <f t="shared" si="2"/>
-        <v>2.6853950590746137E-2</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>121</v>
+        <v>2.904861409551333E-2</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D15" s="8">
         <v>0.38</v>
@@ -1493,19 +1493,19 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" si="2"/>
-        <v>4.9660676037740206E-3</v>
-      </c>
-      <c r="I15" s="36" t="s">
-        <v>121</v>
+        <v>5.3719239896111663E-3</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1525,22 +1525,22 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>1.678986672705917E-2</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>122</v>
+        <v>1.8162033836373791E-2</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>119</v>
       </c>
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8">
         <v>11.4</v>
@@ -1557,25 +1557,25 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>0.1022638071073784</v>
-      </c>
-      <c r="I17" s="36" t="s">
-        <v>121</v>
+        <v>0.110621409634377</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D18" s="8">
         <v>0.99</v>
@@ -1592,23 +1592,23 @@
       </c>
       <c r="H18" s="13">
         <f t="shared" si="2"/>
-        <v>8.2407933424945706E-3</v>
-      </c>
-      <c r="I18" s="36"/>
+        <v>8.9142796639199804E-3</v>
+      </c>
+      <c r="I18" s="33"/>
       <c r="J18" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D19" s="8">
         <v>3.2</v>
@@ -1625,23 +1625,23 @@
       </c>
       <c r="H19" s="13">
         <f t="shared" si="2"/>
-        <v>3.0379258822806874E-2</v>
-      </c>
-      <c r="I19" s="36"/>
+        <v>3.2862031345046727E-2</v>
+      </c>
+      <c r="I19" s="33"/>
       <c r="J19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D20" s="8">
         <v>0.27</v>
@@ -1658,23 +1658,23 @@
       </c>
       <c r="H20" s="13">
         <f t="shared" si="2"/>
-        <v>2.1963453580942588E-3</v>
-      </c>
-      <c r="I20" s="36"/>
+        <v>2.3758436775309292E-3</v>
+      </c>
+      <c r="I20" s="33"/>
       <c r="J20" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D21" s="6">
         <v>1.54</v>
@@ -1691,20 +1691,20 @@
       </c>
       <c r="H21" s="13">
         <f t="shared" si="2"/>
-        <v>1.2894982304485681E-2</v>
-      </c>
-      <c r="I21" s="36"/>
+        <v>1.3948836446454116E-2</v>
+      </c>
+      <c r="I21" s="33"/>
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D22" s="8">
         <v>0.25</v>
@@ -1721,23 +1721,23 @@
       </c>
       <c r="H22" s="13">
         <f t="shared" si="2"/>
-        <v>2.9988330940664376E-3</v>
-      </c>
-      <c r="I22" s="36"/>
+        <v>3.2439154526637481E-3</v>
+      </c>
+      <c r="I22" s="33"/>
       <c r="J22" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D23" s="15">
         <v>0.1</v>
@@ -1746,28 +1746,28 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F23" s="16">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="H23" s="13">
         <f t="shared" si="2"/>
-        <v>1.43943988515189E-2</v>
-      </c>
-      <c r="I23" s="36"/>
+        <v>1.0380529448523993E-2</v>
+      </c>
+      <c r="I23" s="33"/>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="15">
         <v>0.1</v>
@@ -1776,47 +1776,47 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F24" s="16">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="H24" s="13">
         <f t="shared" si="2"/>
-        <v>1.1995332376265751E-3</v>
-      </c>
-      <c r="I24" s="36"/>
+        <v>5.1902647242619967E-3</v>
+      </c>
+      <c r="I24" s="33"/>
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="A25" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="19">
         <f>SUM(G2:G24)</f>
-        <v>83.36575999999998</v>
+        <v>77.067359999999994</v>
       </c>
       <c r="H25" s="32"/>
-      <c r="I25" s="37"/>
+      <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G26" s="19">
         <f>G25</f>
-        <v>83.36575999999998</v>
+        <v>77.067359999999994</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F27" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G27" s="19">
         <f>525/100</f>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F28" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G28" s="19">
         <v>5</v>
@@ -1833,14 +1833,14 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F29" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G29" s="21">
         <f>G26+G27+G28</f>
-        <v>93.61575999999998</v>
+        <v>87.317359999999994</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1848,30 +1848,30 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H34" s="10">
         <v>525</v>
@@ -1879,50 +1879,50 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36"/>
       <c r="E36" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D37"/>
       <c r="E37" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D40" s="8">
         <v>2.59</v>
@@ -1933,13 +1933,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D41" s="8">
         <v>0.95</v>
@@ -1950,20 +1950,20 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>6</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D46" s="8">
         <v>0.44</v>
@@ -2017,19 +2017,19 @@
       </c>
       <c r="H46" s="13">
         <f>G46/$G$26</f>
-        <v>2.2731154853023595E-3</v>
-      </c>
-      <c r="I46" s="36"/>
+        <v>2.458887913119121E-3</v>
+      </c>
+      <c r="I46" s="33"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D47" s="8">
         <v>0.22</v>
@@ -2047,13 +2047,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D48" s="8">
         <v>0.1</v>
@@ -2109,29 +2109,29 @@
     <hyperlink ref="A44" r:id="rId5" xr:uid="{7A52F621-53DC-4944-A105-9D5D48BD709B}"/>
     <hyperlink ref="A45" r:id="rId6" display="https://www.digikey.com/product-detail/en/texas-instruments/HDC2010YPAR/296-47774-6-ND/8133296" xr:uid="{A59B6D7E-18A9-46DD-B79B-3216C251B120}"/>
     <hyperlink ref="A46" r:id="rId7" xr:uid="{5D40EBFA-38D8-4D85-A69A-77A340615339}"/>
-    <hyperlink ref="A2" r:id="rId8" display="https://www.digikey.com/product-detail/en/microchip-technology/PIC32MX795F512L-80I-PT/PIC32MX795F512L-80I-PT-ND/2184451" xr:uid="{96F50DC8-1156-44BD-A100-CECEF0DBA608}"/>
-    <hyperlink ref="A4" r:id="rId9" display="https://www.digikey.com/product-detail/en/stmicroelectronics/LIS3DHTR/497-10613-1-ND/2334355" xr:uid="{75FD6DE8-E3E6-488A-80DA-A82A7415BE34}"/>
-    <hyperlink ref="A5" r:id="rId10" display="CAM-M8" xr:uid="{AAA52117-BA88-47F2-8CEE-882690036EF1}"/>
-    <hyperlink ref="A6" r:id="rId11" xr:uid="{B7E4E087-B402-4FDC-949C-298F88573ED0}"/>
-    <hyperlink ref="A9" r:id="rId12" xr:uid="{BCB74108-468A-49FE-9C12-37C2BA4FC058}"/>
-    <hyperlink ref="A47" r:id="rId13" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
-    <hyperlink ref="A48" r:id="rId14" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
-    <hyperlink ref="A11" r:id="rId15" xr:uid="{00FD8348-3D5C-4D08-B5A1-80F726E66E33}"/>
-    <hyperlink ref="A16" r:id="rId16" display="https://www.digikey.com/product-detail/en/texas-instruments/DRV8872DDAR/296-42661-1-ND/5455926" xr:uid="{6114D03B-D4DA-4FBF-9B1C-C3B7AD098BA9}"/>
-    <hyperlink ref="A17" r:id="rId17" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD7799BRUZ-REEL/AD7799BRUZ-REELCT-ND/4135565" xr:uid="{4B1FE711-B41B-4C95-9AFF-964E590FAEA9}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{C8A12CB4-8BD6-400D-8778-CB90C34529A8}"/>
-    <hyperlink ref="A18" r:id="rId19" xr:uid="{DA75B542-D86D-4B8B-A010-0E90403DB631}"/>
-    <hyperlink ref="A14" r:id="rId20" xr:uid="{7F96FA14-D697-422E-905A-991475B71057}"/>
-    <hyperlink ref="A8" r:id="rId21" xr:uid="{9849B45B-0C58-488D-BA9E-5D0A918112A3}"/>
-    <hyperlink ref="A3" r:id="rId22" xr:uid="{0D2ADA9B-1007-4C76-91DB-7B12AE9573EA}"/>
-    <hyperlink ref="A21" r:id="rId23" xr:uid="{1403372D-5EBE-4749-8D7B-B82E7BCD587C}"/>
-    <hyperlink ref="A7" r:id="rId24" xr:uid="{97352714-91EF-4428-A3E4-A04998CB3C31}"/>
-    <hyperlink ref="A20" r:id="rId25" xr:uid="{DB300913-E56B-4B4B-8B6B-45D99AE75B3D}"/>
-    <hyperlink ref="A13" r:id="rId26" xr:uid="{2B494103-7B58-418F-8039-3EE2EE0764D5}"/>
-    <hyperlink ref="A12" r:id="rId27" xr:uid="{FC62576B-0341-4AB6-A60F-37AA4F9AC5C1}"/>
-    <hyperlink ref="A22" r:id="rId28" xr:uid="{143742D2-F4BE-4740-B25E-8DB03D19A806}"/>
-    <hyperlink ref="A10" r:id="rId29" xr:uid="{DCAF167F-0EB9-4809-861C-A6BC048ADE48}"/>
-    <hyperlink ref="A15" r:id="rId30" xr:uid="{3865BBCF-4D2B-487F-B6E7-CF7AB8CCA0F5}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://www.digikey.com/product-detail/en/stmicroelectronics/LIS3DHTR/497-10613-1-ND/2334355" xr:uid="{75FD6DE8-E3E6-488A-80DA-A82A7415BE34}"/>
+    <hyperlink ref="A6" r:id="rId9" xr:uid="{B7E4E087-B402-4FDC-949C-298F88573ED0}"/>
+    <hyperlink ref="A9" r:id="rId10" xr:uid="{BCB74108-468A-49FE-9C12-37C2BA4FC058}"/>
+    <hyperlink ref="A47" r:id="rId11" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
+    <hyperlink ref="A48" r:id="rId12" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{00FD8348-3D5C-4D08-B5A1-80F726E66E33}"/>
+    <hyperlink ref="A16" r:id="rId14" display="https://www.digikey.com/product-detail/en/texas-instruments/DRV8872DDAR/296-42661-1-ND/5455926" xr:uid="{6114D03B-D4DA-4FBF-9B1C-C3B7AD098BA9}"/>
+    <hyperlink ref="A17" r:id="rId15" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD7799BRUZ-REEL/AD7799BRUZ-REELCT-ND/4135565" xr:uid="{4B1FE711-B41B-4C95-9AFF-964E590FAEA9}"/>
+    <hyperlink ref="A19" r:id="rId16" xr:uid="{C8A12CB4-8BD6-400D-8778-CB90C34529A8}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{DA75B542-D86D-4B8B-A010-0E90403DB631}"/>
+    <hyperlink ref="A14" r:id="rId18" xr:uid="{7F96FA14-D697-422E-905A-991475B71057}"/>
+    <hyperlink ref="A8" r:id="rId19" xr:uid="{9849B45B-0C58-488D-BA9E-5D0A918112A3}"/>
+    <hyperlink ref="A3" r:id="rId20" xr:uid="{0D2ADA9B-1007-4C76-91DB-7B12AE9573EA}"/>
+    <hyperlink ref="A21" r:id="rId21" xr:uid="{1403372D-5EBE-4749-8D7B-B82E7BCD587C}"/>
+    <hyperlink ref="A7" r:id="rId22" xr:uid="{97352714-91EF-4428-A3E4-A04998CB3C31}"/>
+    <hyperlink ref="A20" r:id="rId23" xr:uid="{DB300913-E56B-4B4B-8B6B-45D99AE75B3D}"/>
+    <hyperlink ref="A13" r:id="rId24" xr:uid="{2B494103-7B58-418F-8039-3EE2EE0764D5}"/>
+    <hyperlink ref="A12" r:id="rId25" xr:uid="{FC62576B-0341-4AB6-A60F-37AA4F9AC5C1}"/>
+    <hyperlink ref="A22" r:id="rId26" xr:uid="{143742D2-F4BE-4740-B25E-8DB03D19A806}"/>
+    <hyperlink ref="A10" r:id="rId27" xr:uid="{DCAF167F-0EB9-4809-861C-A6BC048ADE48}"/>
+    <hyperlink ref="A15" r:id="rId28" xr:uid="{3865BBCF-4D2B-487F-B6E7-CF7AB8CCA0F5}"/>
+    <hyperlink ref="A2" r:id="rId29" xr:uid="{02B5AE4F-DA28-4C1B-8D23-D7D5A1AB54B2}"/>
+    <hyperlink ref="A5" r:id="rId30" xr:uid="{E8A4A89C-2D9E-4474-A296-E1633BC9D021}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>

</xml_diff>

<commit_message>
Updates ESD protection diodes
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3DF27164-0875-427B-9E38-2D9A082690D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF25DF71-42D2-4E0C-AAEE-8FAEF83C4468}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="175">
   <si>
     <t>Part Number</t>
   </si>
@@ -209,12 +209,6 @@
     <t>MCU Oscillator</t>
   </si>
   <si>
-    <t>0.1uF, 1uF, 10uF</t>
-  </si>
-  <si>
-    <t>10k, 2.2k, 100, 0</t>
-  </si>
-  <si>
     <t>Revision Date</t>
   </si>
   <si>
@@ -377,24 +371,9 @@
     <t>Total</t>
   </si>
   <si>
-    <t>NEW PCK?</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>74LVC125ABQ</t>
-  </si>
-  <si>
     <t>Nexperia</t>
   </si>
   <si>
-    <t>PIC32MX795F512L-80I/BG</t>
-  </si>
-  <si>
     <t>MAX2771ETI+</t>
   </si>
   <si>
@@ -425,9 +404,6 @@
     <t>100uF &gt;25V</t>
   </si>
   <si>
-    <t>Motor and ADC Bulk</t>
-  </si>
-  <si>
     <t>MF-CAP-6.3MM-100uF</t>
   </si>
   <si>
@@ -443,15 +419,6 @@
     <t>MF-CAP-0402-27pF</t>
   </si>
   <si>
-    <t>MF-CAP-0603-1uF</t>
-  </si>
-  <si>
-    <t>MF-CAP-0603-0.1uF</t>
-  </si>
-  <si>
-    <t>GRM0335C1H100JA01D</t>
-  </si>
-  <si>
     <t>MF-LED-0805-GREEN</t>
   </si>
   <si>
@@ -461,9 +428,6 @@
     <t>LED current limit</t>
   </si>
   <si>
-    <t>MF-RES-0603-60.4</t>
-  </si>
-  <si>
     <t>60 ohm</t>
   </si>
   <si>
@@ -509,9 +473,6 @@
     <t>560pF</t>
   </si>
   <si>
-    <t>Buck Converter</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -539,13 +500,55 @@
     <t>MF-CAP-0805-0.1uF</t>
   </si>
   <si>
-    <t>LCD Driver Anode Rail</t>
-  </si>
-  <si>
     <t>3SMAJ5935B-TP</t>
   </si>
   <si>
     <t>Screen zener diode</t>
+  </si>
+  <si>
+    <t>MF-RES-0402-60.4</t>
+  </si>
+  <si>
+    <t>MF-CAP-0402-0.1uF</t>
+  </si>
+  <si>
+    <t>MF-CAP-0402-1uF</t>
+  </si>
+  <si>
+    <t>LCD Driver &amp; Motor Driver</t>
+  </si>
+  <si>
+    <t>Motor &amp; ADC Bulk</t>
+  </si>
+  <si>
+    <t>CL05B471JB5NNNC</t>
+  </si>
+  <si>
+    <t>470pF</t>
+  </si>
+  <si>
+    <t>5V Regulator</t>
+  </si>
+  <si>
+    <t>3V3 Buck Converter</t>
+  </si>
+  <si>
+    <t>o603</t>
+  </si>
+  <si>
+    <t>can 6.3mm</t>
+  </si>
+  <si>
+    <t>o805</t>
+  </si>
+  <si>
+    <t>CL21A106KQCLRNC</t>
+  </si>
+  <si>
+    <t>PIC32MX795F512L-80I/PT</t>
+  </si>
+  <si>
+    <t>74HCT125D</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -707,15 +710,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -726,7 +720,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -762,7 +756,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -773,9 +766,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="2" borderId="2" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -806,15 +796,6 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -824,11 +805,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -836,6 +812,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1131,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,15 +1126,14 @@
     <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="35" customWidth="1"/>
-    <col min="10" max="10" width="62.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="26" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.7109375" customWidth="1"/>
+    <col min="9" max="9" width="62.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1144,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1180,28 +1158,25 @@
       <c r="H1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>102</v>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>122</v>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>173</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1219,39 +1194,36 @@
         <v>1</v>
       </c>
       <c r="G2" s="8">
-        <f t="shared" ref="G2:G24" si="0">F2*E2</f>
+        <f t="shared" ref="G2:G22" si="0">F2*E2</f>
         <v>8.3739000000000008</v>
       </c>
       <c r="H2" s="13">
-        <f t="shared" ref="H2:H11" si="1">G2/$G$26</f>
-        <v>0.10865689443624385</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="14">
+        <f t="shared" ref="H2:H11" si="1">G2/$G$24</f>
+        <v>0.11048329299558697</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="14">
         <v>43413</v>
       </c>
-      <c r="M2" s="8">
+      <c r="L2" s="8">
         <v>98.69</v>
       </c>
-      <c r="N2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>78</v>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="8">
         <v>1.66</v>
@@ -1268,27 +1240,24 @@
       </c>
       <c r="H3" s="13">
         <f t="shared" si="1"/>
-        <v>1.9982519188408689E-2</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="14">
+        <v>2.0318402561913078E-2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="22"/>
+      <c r="K3" s="14">
         <v>43383</v>
       </c>
-      <c r="M3" s="8">
+      <c r="L3" s="8">
         <v>80.599999999999994</v>
       </c>
-      <c r="N3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="M3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1312,25 +1281,22 @@
       </c>
       <c r="H4" s="13">
         <f t="shared" si="1"/>
-        <v>9.2023393561165203E-3</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>123</v>
+        <v>9.3570201927978928E-3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D5" s="8">
         <v>7.36</v>
@@ -1347,18 +1313,15 @@
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>7.1002821427904123E-2</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+        <v>7.2196297934278161E-2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1382,17 +1345,16 @@
       </c>
       <c r="H6" s="13">
         <f t="shared" si="1"/>
-        <v>3.3412329162436603E-3</v>
-      </c>
-      <c r="I6" s="33"/>
-      <c r="K6" s="24"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>91</v>
+        <v>3.3973952335666349E-3</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -1412,16 +1374,13 @@
       </c>
       <c r="H7" s="13">
         <f t="shared" si="1"/>
-        <v>4.5985745456961291E-3</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>74</v>
+        <v>4.6758713428194766E-3</v>
+      </c>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
@@ -1444,21 +1403,18 @@
       </c>
       <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>0.4407858268403122</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J8" s="2" t="s">
+        <v>0.44819493422642831</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1479,17 +1435,16 @@
       </c>
       <c r="H9" s="13">
         <f t="shared" si="1"/>
-        <v>7.5779162540406224E-3</v>
-      </c>
-      <c r="I9" s="33"/>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>113</v>
+        <v>7.7052923897291282E-3</v>
+      </c>
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>35</v>
@@ -1509,16 +1464,15 @@
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>4.6011696780582596E-2</v>
-      </c>
-      <c r="I10" s="33"/>
-      <c r="K10" s="24"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+        <v>4.6785100963989461E-2</v>
+      </c>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1539,22 +1493,19 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="1"/>
-        <v>3.666532757836781E-2</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>99</v>
+        <v>3.7281629947531023E-2</v>
+      </c>
+      <c r="J11" s="22"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="8">
         <v>0.47</v>
@@ -1570,20 +1521,17 @@
         <v>0.31950000000000001</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="K12" s="24"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="16" t="s">
+      <c r="J12" s="22"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" s="8">
         <v>0.77</v>
@@ -1599,22 +1547,19 @@
         <v>0.60955999999999999</v>
       </c>
       <c r="H13" s="13">
-        <f t="shared" ref="H13:H24" si="2">G13/$G$26</f>
-        <v>7.9094444133028571E-3</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J13" s="2" t="s">
+        <f t="shared" ref="H13:H22" si="2">G13/$G$24</f>
+        <v>8.0423931595063215E-3</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="J13" s="22"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1635,53 +1580,47 @@
       </c>
       <c r="H14" s="13">
         <f t="shared" si="2"/>
-        <v>2.904861409551333E-2</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="16" t="s">
+        <v>2.9536888191788836E-2</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="22"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D15" s="8">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="E15" s="8">
-        <v>0.20699999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
-        <v>0.41399999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="H15" s="13">
         <f t="shared" si="2"/>
-        <v>5.3719239896111663E-3</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+        <v>4.4858810850976925E-3</v>
+      </c>
+      <c r="J15" s="22"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1702,19 +1641,16 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>1.8162033836373791E-2</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+        <v>1.8467316925915411E-2</v>
+      </c>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>115</v>
+      <c r="B17" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>46</v>
@@ -1734,22 +1670,19 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>0.110621409634377</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+        <v>0.11248082945524517</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>93</v>
+      <c r="B18" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>41</v>
@@ -1769,19 +1702,18 @@
       </c>
       <c r="H18" s="13">
         <f t="shared" si="2"/>
-        <v>8.9142796639199804E-3</v>
-      </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="2" t="s">
+        <v>9.064118545476809E-3</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="J18" s="22"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1802,23 +1734,22 @@
       </c>
       <c r="H19" s="13">
         <f t="shared" si="2"/>
-        <v>3.2862031345046727E-2</v>
-      </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="2" t="s">
+        <v>3.3414404639139896E-2</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="16" t="s">
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="8">
         <v>0.27</v>
@@ -1835,23 +1766,22 @@
       </c>
       <c r="H20" s="13">
         <f t="shared" si="2"/>
-        <v>2.3758436775309292E-3</v>
-      </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="2" t="s">
+        <v>2.4157789020040812E-3</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K20" s="24"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D21" s="6">
         <v>1.54</v>
@@ -1868,20 +1798,19 @@
       </c>
       <c r="H21" s="13">
         <f t="shared" si="2"/>
-        <v>1.3948836446454116E-2</v>
-      </c>
-      <c r="I21" s="33"/>
-      <c r="K21" s="24"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+        <v>1.4183300489647116E-2</v>
+      </c>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>109</v>
       </c>
       <c r="D22" s="8">
         <v>0.25</v>
@@ -1898,360 +1827,297 @@
       </c>
       <c r="H22" s="13">
         <f t="shared" si="2"/>
-        <v>3.2439154526637481E-3</v>
-      </c>
-      <c r="I22" s="33"/>
-      <c r="J22" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K22" s="24"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="15">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F23" s="16">
-        <v>200</v>
-      </c>
-      <c r="G23" s="8">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="H23" s="13">
-        <f t="shared" si="2"/>
-        <v>1.0380529448523993E-2</v>
-      </c>
-      <c r="I23" s="33"/>
-      <c r="K23" s="24"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="15">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F24" s="16">
-        <v>100</v>
-      </c>
-      <c r="G24" s="8">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="H24" s="13">
-        <f t="shared" si="2"/>
-        <v>5.1902647242619967E-3</v>
-      </c>
-      <c r="I24" s="33"/>
-      <c r="K24" s="24"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="19">
-        <f>SUM(G2:G24)</f>
-        <v>77.067359999999994</v>
-      </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="34"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="19">
-        <f>G25</f>
-        <v>77.067359999999994</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="19">
+        <v>3.2984419743365386E-3</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="18">
+        <f>SUM(G2:G22)</f>
+        <v>75.793359999999993</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="18">
+        <f>G23</f>
+        <v>75.793359999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="18">
         <f>525/100</f>
         <v>5.25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="19">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="21">
-        <f>G26+G27+G28</f>
-        <v>87.317359999999994</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K31" s="23"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="19">
+        <f>G24+G25+G26</f>
+        <v>86.043359999999993</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="21"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="10">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D34"/>
       <c r="E34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="10">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D35"/>
       <c r="E35" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36"/>
-      <c r="E36" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37"/>
-      <c r="E37" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D38" s="8">
         <v>2.59</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E38" s="8">
         <v>2.0739000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0.71830000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="8">
-        <v>0.95</v>
-      </c>
-      <c r="E41" s="8">
-        <v>0.71830000000000005</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>75</v>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="6">
+        <v>5.78</v>
+      </c>
+      <c r="E42" s="8">
+        <v>4.7998000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="8">
+        <v>3.35</v>
+      </c>
+      <c r="E43" s="8">
+        <v>1.8204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="6">
-        <v>5.78</v>
+        <v>16</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0.44</v>
       </c>
       <c r="E44" s="8">
-        <v>4.7998000000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>10</v>
+        <v>0.1895</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="8">
+        <f>F44*E44</f>
+        <v>0.1895</v>
+      </c>
+      <c r="H44" s="13">
+        <f>G44/$G$24</f>
+        <v>2.5002190165470963E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D45" s="8">
-        <v>3.35</v>
+        <v>0.22</v>
       </c>
       <c r="E45" s="8">
-        <v>1.8204</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>17</v>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F45" s="2">
+        <v>5</v>
+      </c>
+      <c r="G45" s="8">
+        <f>F45*E45</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D46" s="8">
-        <v>0.44</v>
+        <v>0.1</v>
       </c>
       <c r="E46" s="8">
-        <v>0.1895</v>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F46" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G46" s="8">
         <f>F46*E46</f>
-        <v>0.1895</v>
-      </c>
-      <c r="H46" s="13">
-        <f>G46/$G$26</f>
-        <v>2.458887913119121E-3</v>
-      </c>
-      <c r="I46" s="33"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="E47" s="8">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F47" s="2">
-        <v>5</v>
-      </c>
-      <c r="G47" s="8">
-        <f>F47*E47</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D48" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E48" s="8">
-        <v>6.0199999999999997E-2</v>
-      </c>
-      <c r="F48" s="2">
-        <v>4</v>
-      </c>
-      <c r="G48" s="8">
-        <f>F48*E48</f>
         <v>0.24079999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A23:F23"/>
   </mergeCells>
-  <conditionalFormatting sqref="H46:I46">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="H44">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2264,8 +2130,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I25">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="H2:H23">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2279,18 +2145,18 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A42" r:id="rId1" xr:uid="{5678B9E6-DE86-401B-BDAE-7D9F6469FDE3}"/>
-    <hyperlink ref="A43" r:id="rId2" xr:uid="{7E8CB0A3-F47D-4B54-B720-D9CD7DF2F8EE}"/>
-    <hyperlink ref="A40" r:id="rId3" xr:uid="{653FFE94-4D7F-4394-B0B2-10332AAC8742}"/>
-    <hyperlink ref="A41" r:id="rId4" display="https://www.digikey.com/product-detail/en/molex-llc/0522710679/WM7955CT-ND/1960704" xr:uid="{C446B2E0-C0B0-47BA-BB19-2A932AEA1D87}"/>
-    <hyperlink ref="A44" r:id="rId5" xr:uid="{7A52F621-53DC-4944-A105-9D5D48BD709B}"/>
-    <hyperlink ref="A45" r:id="rId6" display="https://www.digikey.com/product-detail/en/texas-instruments/HDC2010YPAR/296-47774-6-ND/8133296" xr:uid="{A59B6D7E-18A9-46DD-B79B-3216C251B120}"/>
-    <hyperlink ref="A46" r:id="rId7" xr:uid="{5D40EBFA-38D8-4D85-A69A-77A340615339}"/>
+    <hyperlink ref="A40" r:id="rId1" xr:uid="{5678B9E6-DE86-401B-BDAE-7D9F6469FDE3}"/>
+    <hyperlink ref="A41" r:id="rId2" xr:uid="{7E8CB0A3-F47D-4B54-B720-D9CD7DF2F8EE}"/>
+    <hyperlink ref="A38" r:id="rId3" xr:uid="{653FFE94-4D7F-4394-B0B2-10332AAC8742}"/>
+    <hyperlink ref="A39" r:id="rId4" display="https://www.digikey.com/product-detail/en/molex-llc/0522710679/WM7955CT-ND/1960704" xr:uid="{C446B2E0-C0B0-47BA-BB19-2A932AEA1D87}"/>
+    <hyperlink ref="A42" r:id="rId5" xr:uid="{7A52F621-53DC-4944-A105-9D5D48BD709B}"/>
+    <hyperlink ref="A43" r:id="rId6" display="https://www.digikey.com/product-detail/en/texas-instruments/HDC2010YPAR/296-47774-6-ND/8133296" xr:uid="{A59B6D7E-18A9-46DD-B79B-3216C251B120}"/>
+    <hyperlink ref="A44" r:id="rId7" xr:uid="{5D40EBFA-38D8-4D85-A69A-77A340615339}"/>
     <hyperlink ref="A4" r:id="rId8" display="https://www.digikey.com/product-detail/en/stmicroelectronics/LIS3DHTR/497-10613-1-ND/2334355" xr:uid="{75FD6DE8-E3E6-488A-80DA-A82A7415BE34}"/>
     <hyperlink ref="A6" r:id="rId9" xr:uid="{B7E4E087-B402-4FDC-949C-298F88573ED0}"/>
     <hyperlink ref="A9" r:id="rId10" xr:uid="{BCB74108-468A-49FE-9C12-37C2BA4FC058}"/>
-    <hyperlink ref="A47" r:id="rId11" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
-    <hyperlink ref="A48" r:id="rId12" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
+    <hyperlink ref="A45" r:id="rId11" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
+    <hyperlink ref="A46" r:id="rId12" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
     <hyperlink ref="A11" r:id="rId13" xr:uid="{00FD8348-3D5C-4D08-B5A1-80F726E66E33}"/>
     <hyperlink ref="A16" r:id="rId14" display="https://www.digikey.com/product-detail/en/texas-instruments/DRV8872DDAR/296-42661-1-ND/5455926" xr:uid="{6114D03B-D4DA-4FBF-9B1C-C3B7AD098BA9}"/>
     <hyperlink ref="A17" r:id="rId15" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD7799BRUZ-REEL/AD7799BRUZ-REELCT-ND/4135565" xr:uid="{4B1FE711-B41B-4C95-9AFF-964E590FAEA9}"/>
@@ -2306,9 +2172,9 @@
     <hyperlink ref="A12" r:id="rId25" xr:uid="{FC62576B-0341-4AB6-A60F-37AA4F9AC5C1}"/>
     <hyperlink ref="A22" r:id="rId26" xr:uid="{143742D2-F4BE-4740-B25E-8DB03D19A806}"/>
     <hyperlink ref="A10" r:id="rId27" xr:uid="{DCAF167F-0EB9-4809-861C-A6BC048ADE48}"/>
-    <hyperlink ref="A15" r:id="rId28" xr:uid="{3865BBCF-4D2B-487F-B6E7-CF7AB8CCA0F5}"/>
-    <hyperlink ref="A2" r:id="rId29" xr:uid="{02B5AE4F-DA28-4C1B-8D23-D7D5A1AB54B2}"/>
-    <hyperlink ref="A5" r:id="rId30" xr:uid="{E8A4A89C-2D9E-4474-A296-E1633BC9D021}"/>
+    <hyperlink ref="A5" r:id="rId28" xr:uid="{E8A4A89C-2D9E-4474-A296-E1633BC9D021}"/>
+    <hyperlink ref="A2" r:id="rId29" xr:uid="{6353ACF5-8899-4C18-9701-ACEEF9533176}"/>
+    <hyperlink ref="A15" r:id="rId30" display="74HC125D" xr:uid="{E676067A-C1FC-4C53-866B-6F5E4C42B0DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>
@@ -2324,7 +2190,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H46:I46</xm:sqref>
+          <xm:sqref>H44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E5B5708F-AF4E-472B-86D4-E608850ED8C2}">
@@ -2335,7 +2201,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H2:I25</xm:sqref>
+          <xm:sqref>H2:H23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2345,260 +2211,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A2BDBB-E2E5-4A1F-91BC-824E3760DD54}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" style="38" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="38" customWidth="1"/>
+    <col min="1" max="1" width="29" style="33" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="33" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="B10" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="38" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="33" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="B19" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>153</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
-        <v>172</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-6.3MM-100uF" xr:uid="{AD0A0613-7EE3-4DFC-BB9B-AB85EE1179A0}"/>
+    <hyperlink ref="A9" r:id="rId1" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-6.3MM-100uF" xr:uid="{AD0A0613-7EE3-4DFC-BB9B-AB85EE1179A0}"/>
     <hyperlink ref="A3" r:id="rId2" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-IND-1210-10uH" xr:uid="{EA279B76-C069-48E6-875D-21C36761CFB1}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{EE56DCE3-3FAF-45AF-BE62-D47532FE15DC}"/>
-    <hyperlink ref="A9" r:id="rId4" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0402-27pF" xr:uid="{CDD7C369-2780-40A2-8950-7C38324873F5}"/>
-    <hyperlink ref="A6" r:id="rId5" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0603-1uF" xr:uid="{0CD3D40E-B416-45C2-A1DD-7FFD6135FF9B}"/>
-    <hyperlink ref="A4" r:id="rId6" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0603-0.1uF" xr:uid="{DAEFAB96-80DF-456C-93C0-38F7378F2790}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{41E8E22B-820D-4E1A-B141-1D7654DED6F3}"/>
-    <hyperlink ref="A11" r:id="rId8" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-LED-0805-GREEN" xr:uid="{7DFF6B3D-787F-47A9-A6D3-729E7FCBC3A0}"/>
-    <hyperlink ref="A12" r:id="rId9" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0603-60.4" xr:uid="{DBB9DB0F-8C02-4381-A7CC-9101709382EE}"/>
-    <hyperlink ref="A13" r:id="rId10" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-10" xr:uid="{2BD5AAE5-D696-4B7F-A0BF-3F32D3A5FBB6}"/>
-    <hyperlink ref="A14" r:id="rId11" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-100" xr:uid="{AB9FD5BC-6FDD-4BDE-BE37-A7B25174F77D}"/>
-    <hyperlink ref="A15" r:id="rId12" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-2K" xr:uid="{704352B8-9840-49D3-AEF2-9C6C28C45000}"/>
-    <hyperlink ref="A16" r:id="rId13" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-10K" xr:uid="{7D8C8875-6DA7-4EFE-99F2-BECC2831B987}"/>
-    <hyperlink ref="A17" r:id="rId14" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0603-0" xr:uid="{C08C6073-743C-40FD-82E3-3A1BECE5A666}"/>
-    <hyperlink ref="A18" r:id="rId15" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-22" xr:uid="{4C316F1E-6CAA-49E3-8090-9418F20A45F4}"/>
-    <hyperlink ref="A10" r:id="rId16" xr:uid="{5FA9567C-3160-4F07-AD08-B51798CCAF4B}"/>
-    <hyperlink ref="A21" r:id="rId17" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-SW-TACT-6MM" xr:uid="{C3AA1A7F-68D3-4682-B6F9-55C1C1369C0D}"/>
-    <hyperlink ref="A19" r:id="rId18" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-220" xr:uid="{E359756A-0415-431F-A1A9-0662DED44B67}"/>
-    <hyperlink ref="A24" r:id="rId19" xr:uid="{1E01E320-2845-4BB6-AC28-9EA672CB4CFD}"/>
-    <hyperlink ref="A23" r:id="rId20" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-DIO-SMA-B140" xr:uid="{835424EF-0BAF-42F8-B127-DD19F5270BED}"/>
-    <hyperlink ref="A5" r:id="rId21" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0805-0.1uF" xr:uid="{94CB8BA7-D7E0-4A91-A2F6-202B89E8577D}"/>
-    <hyperlink ref="A22" r:id="rId22" xr:uid="{EC2B025F-0EEE-4694-8FD7-481DE501171B}"/>
+    <hyperlink ref="A10" r:id="rId4" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0402-27pF" xr:uid="{CDD7C369-2780-40A2-8950-7C38324873F5}"/>
+    <hyperlink ref="A14" r:id="rId5" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-LED-0805-GREEN" xr:uid="{7DFF6B3D-787F-47A9-A6D3-729E7FCBC3A0}"/>
+    <hyperlink ref="A17" r:id="rId6" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-10" xr:uid="{2BD5AAE5-D696-4B7F-A0BF-3F32D3A5FBB6}"/>
+    <hyperlink ref="A18" r:id="rId7" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-100" xr:uid="{AB9FD5BC-6FDD-4BDE-BE37-A7B25174F77D}"/>
+    <hyperlink ref="A19" r:id="rId8" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-2K" xr:uid="{704352B8-9840-49D3-AEF2-9C6C28C45000}"/>
+    <hyperlink ref="A20" r:id="rId9" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-10K" xr:uid="{7D8C8875-6DA7-4EFE-99F2-BECC2831B987}"/>
+    <hyperlink ref="A21" r:id="rId10" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0603-0" xr:uid="{C08C6073-743C-40FD-82E3-3A1BECE5A666}"/>
+    <hyperlink ref="A22" r:id="rId11" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-22" xr:uid="{4C316F1E-6CAA-49E3-8090-9418F20A45F4}"/>
+    <hyperlink ref="A11" r:id="rId12" xr:uid="{5FA9567C-3160-4F07-AD08-B51798CCAF4B}"/>
+    <hyperlink ref="A25" r:id="rId13" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-SW-TACT-6MM" xr:uid="{C3AA1A7F-68D3-4682-B6F9-55C1C1369C0D}"/>
+    <hyperlink ref="A23" r:id="rId14" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-220" xr:uid="{E359756A-0415-431F-A1A9-0662DED44B67}"/>
+    <hyperlink ref="A28" r:id="rId15" xr:uid="{1E01E320-2845-4BB6-AC28-9EA672CB4CFD}"/>
+    <hyperlink ref="A27" r:id="rId16" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-DIO-SMA-B140" xr:uid="{835424EF-0BAF-42F8-B127-DD19F5270BED}"/>
+    <hyperlink ref="A6" r:id="rId17" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0805-0.1uF" xr:uid="{94CB8BA7-D7E0-4A91-A2F6-202B89E8577D}"/>
+    <hyperlink ref="A26" r:id="rId18" xr:uid="{EC2B025F-0EEE-4694-8FD7-481DE501171B}"/>
+    <hyperlink ref="A16" r:id="rId19" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-RES-0402-60.4" xr:uid="{5BFB6755-EEC8-4963-A7DD-9FA4C58D5765}"/>
+    <hyperlink ref="A5" r:id="rId20" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0402-0.1uF" xr:uid="{2FF3BEA1-ED74-4A86-8CE6-B3E6F2CFD2AA}"/>
+    <hyperlink ref="A7" r:id="rId21" tooltip="Open part details in a new window." display="https://factory.macrofab.com/part/MF-CAP-0402-1uF" xr:uid="{24787A0E-3E87-4BF0-92C9-BE5664FB3292}"/>
+    <hyperlink ref="A12" r:id="rId22" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL05B471JB5NNNC/1276-1564-1-ND/3889650" xr:uid="{2568FC0A-181D-4CE6-A3C4-041FEE7F3830}"/>
+    <hyperlink ref="A8" r:id="rId23" xr:uid="{847E7397-91E4-4D91-A7E3-EF26D770E118}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got to PCB layout
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF25DF71-42D2-4E0C-AAEE-8FAEF83C4468}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{870500AA-4E12-4CC9-A815-CB4AFD79983B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
   <si>
     <t>Part Number</t>
   </si>
@@ -83,9 +83,6 @@
     <t>3V Reg</t>
   </si>
   <si>
-    <t>4.3" LCD</t>
-  </si>
-  <si>
     <t>Newhaven Display</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>`</t>
   </si>
   <si>
-    <t>NHD-4.3-480272EF-ASXV#-T</t>
-  </si>
-  <si>
     <t>PIC32MX430F064L-I/PT</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
     <t>ABO, cut up to $2.15, with MAX-M8C</t>
   </si>
   <si>
-    <t>54104-4031</t>
-  </si>
-  <si>
     <t>LCD(-17.63), Temp(-0.28), Tconn(-0.72),TLCD(+0.17)</t>
   </si>
   <si>
@@ -549,6 +540,21 @@
   </si>
   <si>
     <t>74HCT125D</t>
+  </si>
+  <si>
+    <t>7.0" LCD</t>
+  </si>
+  <si>
+    <t>4-1734839-0</t>
+  </si>
+  <si>
+    <t>TE-Connectivity</t>
+  </si>
+  <si>
+    <t>Display Oscillator</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B2-T</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1150,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1156,27 +1162,27 @@
         <v>4</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1194,15 +1200,15 @@
         <v>1</v>
       </c>
       <c r="G2" s="8">
-        <f t="shared" ref="G2:G22" si="0">F2*E2</f>
+        <f t="shared" ref="G2:G23" si="0">F2*E2</f>
         <v>8.3739000000000008</v>
       </c>
       <c r="H2" s="13">
-        <f t="shared" ref="H2:H11" si="1">G2/$G$24</f>
-        <v>0.11048329299558697</v>
+        <f t="shared" ref="H2:H11" si="1">G2/$G$25</f>
+        <v>0.1076828669549046</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="14">
@@ -1212,18 +1218,18 @@
         <v>98.69</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="8">
         <v>1.66</v>
@@ -1240,10 +1246,10 @@
       </c>
       <c r="H3" s="13">
         <f t="shared" si="1"/>
-        <v>2.0318402561913078E-2</v>
+        <v>1.9803390906334335E-2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J3" s="22"/>
       <c r="K3" s="14">
@@ -1253,7 +1259,7 @@
         <v>80.599999999999994</v>
       </c>
       <c r="M3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1281,22 +1287,22 @@
       </c>
       <c r="H4" s="13">
         <f t="shared" si="1"/>
-        <v>9.3570201927978928E-3</v>
+        <v>9.1198472927092929E-3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D5" s="8">
         <v>7.36</v>
@@ -1313,10 +1319,10 @@
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>7.2196297934278161E-2</v>
+        <v>7.0366334441208753E-2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J5" s="29"/>
     </row>
@@ -1345,16 +1351,16 @@
       </c>
       <c r="H6" s="13">
         <f t="shared" si="1"/>
-        <v>3.3973952335666349E-3</v>
+        <v>3.3112812716760329E-3</v>
       </c>
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -1374,48 +1380,48 @@
       </c>
       <c r="H7" s="13">
         <f t="shared" si="1"/>
-        <v>4.6758713428194766E-3</v>
+        <v>4.5573517774057711E-3</v>
       </c>
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="8">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E8" s="8">
-        <v>33.970199999999998</v>
+        <v>38</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>33.970199999999998</v>
+        <v>38</v>
       </c>
       <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>0.44819493422642831</v>
+        <v>0.48865510028617187</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -1435,19 +1441,19 @@
       </c>
       <c r="H9" s="13">
         <f t="shared" si="1"/>
-        <v>7.7052923897291282E-3</v>
+        <v>7.5099859241612435E-3</v>
       </c>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6">
         <v>5.71</v>
@@ -1464,19 +1470,19 @@
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>4.6785100963989461E-2</v>
+        <v>4.5599236463546453E-2</v>
       </c>
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="8">
         <v>3.58</v>
@@ -1493,19 +1499,19 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="1"/>
-        <v>3.7281629947531023E-2</v>
+        <v>3.6336650444174626E-2</v>
       </c>
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D12" s="8">
         <v>0.47</v>
@@ -1525,13 +1531,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D13" s="8">
         <v>0.77</v>
@@ -1547,55 +1553,50 @@
         <v>0.60955999999999999</v>
       </c>
       <c r="H13" s="13">
-        <f t="shared" ref="H13:H22" si="2">G13/$G$24</f>
-        <v>8.0423931595063215E-3</v>
+        <f t="shared" ref="H13:H23" si="2">G13/$G$25</f>
+        <v>7.8385421823799709E-3</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="8">
-        <v>2.6</v>
-      </c>
-      <c r="E14" s="8">
-        <v>2.2387000000000001</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" si="0"/>
-        <v>2.2387000000000001</v>
+        <v>0</v>
       </c>
       <c r="H14" s="13">
         <f t="shared" si="2"/>
-        <v>2.9536888191788836E-2</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D15" s="8">
         <v>0.39</v>
@@ -1612,16 +1613,16 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" si="2"/>
-        <v>4.4858810850976925E-3</v>
+        <v>4.3721772130868013E-3</v>
       </c>
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1641,19 +1642,19 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>1.8467316925915411E-2</v>
+        <v>1.7999224838698809E-2</v>
       </c>
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D17" s="8">
         <v>11.4</v>
@@ -1670,22 +1671,22 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>0.11248082945524517</v>
+        <v>0.10962977174920266</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8">
         <v>0.99</v>
@@ -1702,22 +1703,22 @@
       </c>
       <c r="H18" s="13">
         <f t="shared" si="2"/>
-        <v>9.064118545476809E-3</v>
+        <v>8.8343698393842131E-3</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D19" s="8">
         <v>3.2</v>
@@ -1734,22 +1735,22 @@
       </c>
       <c r="H19" s="13">
         <f t="shared" si="2"/>
-        <v>3.3414404639139896E-2</v>
+        <v>3.2567447906151473E-2</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D20" s="8">
         <v>0.27</v>
@@ -1766,213 +1767,226 @@
       </c>
       <c r="H20" s="13">
         <f t="shared" si="2"/>
-        <v>2.4157789020040812E-3</v>
+        <v>2.3545460226946863E-3</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1.54</v>
+        <v>176</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.27</v>
       </c>
       <c r="E21" s="8">
-        <v>1.075</v>
-      </c>
-      <c r="F21" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="F21" s="24">
         <v>1</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>1.075</v>
+        <v>0.18</v>
       </c>
       <c r="H21" s="13">
         <f t="shared" si="2"/>
-        <v>1.4183300489647116E-2</v>
-      </c>
+        <v>2.3146820539871296E-3</v>
+      </c>
+      <c r="I21" s="24"/>
       <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0.25</v>
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.54</v>
       </c>
       <c r="E22" s="8">
-        <v>0.25</v>
+        <v>1.075</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>1.075</v>
       </c>
       <c r="H22" s="13">
         <f t="shared" si="2"/>
-        <v>3.2984419743365386E-3</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>106</v>
+        <v>1.3823795600200913E-2</v>
       </c>
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="18">
-        <f>SUM(G2:G22)</f>
-        <v>75.793359999999993</v>
-      </c>
-      <c r="H23" s="30"/>
+      <c r="A23" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" si="2"/>
+        <v>3.2148361860932359E-3</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A24" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
       <c r="G24" s="18">
-        <f>G23</f>
-        <v>75.793359999999993</v>
-      </c>
+        <f>SUM(G2:G23)</f>
+        <v>77.76446</v>
+      </c>
+      <c r="H24" s="30"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G25" s="18">
+        <f>G24</f>
+        <v>77.76446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="18">
         <f>525/100</f>
         <v>5.25</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="18">
-        <v>5</v>
-      </c>
-    </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="19">
-        <f>G24+G25+G26</f>
-        <v>86.043359999999993</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J29" s="21"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>85</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G27" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="19">
+        <f>G25+G26+G27</f>
+        <v>88.01446</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="21"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="10">
-        <v>525</v>
+        <v>65</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="H33" s="10">
+        <v>525</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34"/>
+        <v>47</v>
+      </c>
       <c r="E34" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D35"/>
       <c r="E35" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="8">
-        <v>2.59</v>
-      </c>
-      <c r="E38" s="8">
-        <v>2.0739000000000001</v>
+        <v>43</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1980,143 +1994,160 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="8">
+        <v>2.59</v>
+      </c>
+      <c r="E39" s="8">
+        <v>2.0739000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="8">
+      <c r="B40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="8">
         <v>0.95</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E40" s="8">
         <v>0.71830000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="2" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <v>5.78</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E43" s="8">
         <v>4.7998000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D44" s="8">
         <v>3.35</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E44" s="8">
         <v>1.8204</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D45" s="8">
         <v>0.44</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E45" s="8">
         <v>0.1895</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F45" s="2">
         <v>1</v>
-      </c>
-      <c r="G44" s="8">
-        <f>F44*E44</f>
-        <v>0.1895</v>
-      </c>
-      <c r="H44" s="13">
-        <f>G44/$G$24</f>
-        <v>2.5002190165470963E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="E45" s="8">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F45" s="2">
-        <v>5</v>
       </c>
       <c r="G45" s="8">
         <f>F45*E45</f>
-        <v>0.72</v>
+        <v>0.1895</v>
+      </c>
+      <c r="H45" s="13">
+        <f>G45/$G$25</f>
+        <v>2.4368458290586728E-3</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D46" s="8">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="E46" s="8">
-        <v>6.0199999999999997E-2</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F46" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G46" s="8">
         <f>F46*E46</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E47" s="8">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47" s="8">
+        <f>F47*E47</f>
         <v>0.24079999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
   </mergeCells>
-  <conditionalFormatting sqref="H44">
+  <conditionalFormatting sqref="H45">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
@@ -2130,7 +2161,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
@@ -2145,39 +2176,40 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A40" r:id="rId1" xr:uid="{5678B9E6-DE86-401B-BDAE-7D9F6469FDE3}"/>
-    <hyperlink ref="A41" r:id="rId2" xr:uid="{7E8CB0A3-F47D-4B54-B720-D9CD7DF2F8EE}"/>
-    <hyperlink ref="A38" r:id="rId3" xr:uid="{653FFE94-4D7F-4394-B0B2-10332AAC8742}"/>
-    <hyperlink ref="A39" r:id="rId4" display="https://www.digikey.com/product-detail/en/molex-llc/0522710679/WM7955CT-ND/1960704" xr:uid="{C446B2E0-C0B0-47BA-BB19-2A932AEA1D87}"/>
-    <hyperlink ref="A42" r:id="rId5" xr:uid="{7A52F621-53DC-4944-A105-9D5D48BD709B}"/>
-    <hyperlink ref="A43" r:id="rId6" display="https://www.digikey.com/product-detail/en/texas-instruments/HDC2010YPAR/296-47774-6-ND/8133296" xr:uid="{A59B6D7E-18A9-46DD-B79B-3216C251B120}"/>
-    <hyperlink ref="A44" r:id="rId7" xr:uid="{5D40EBFA-38D8-4D85-A69A-77A340615339}"/>
+    <hyperlink ref="A41" r:id="rId1" xr:uid="{5678B9E6-DE86-401B-BDAE-7D9F6469FDE3}"/>
+    <hyperlink ref="A42" r:id="rId2" xr:uid="{7E8CB0A3-F47D-4B54-B720-D9CD7DF2F8EE}"/>
+    <hyperlink ref="A39" r:id="rId3" xr:uid="{653FFE94-4D7F-4394-B0B2-10332AAC8742}"/>
+    <hyperlink ref="A40" r:id="rId4" display="https://www.digikey.com/product-detail/en/molex-llc/0522710679/WM7955CT-ND/1960704" xr:uid="{C446B2E0-C0B0-47BA-BB19-2A932AEA1D87}"/>
+    <hyperlink ref="A43" r:id="rId5" xr:uid="{7A52F621-53DC-4944-A105-9D5D48BD709B}"/>
+    <hyperlink ref="A44" r:id="rId6" display="https://www.digikey.com/product-detail/en/texas-instruments/HDC2010YPAR/296-47774-6-ND/8133296" xr:uid="{A59B6D7E-18A9-46DD-B79B-3216C251B120}"/>
+    <hyperlink ref="A45" r:id="rId7" xr:uid="{5D40EBFA-38D8-4D85-A69A-77A340615339}"/>
     <hyperlink ref="A4" r:id="rId8" display="https://www.digikey.com/product-detail/en/stmicroelectronics/LIS3DHTR/497-10613-1-ND/2334355" xr:uid="{75FD6DE8-E3E6-488A-80DA-A82A7415BE34}"/>
     <hyperlink ref="A6" r:id="rId9" xr:uid="{B7E4E087-B402-4FDC-949C-298F88573ED0}"/>
     <hyperlink ref="A9" r:id="rId10" xr:uid="{BCB74108-468A-49FE-9C12-37C2BA4FC058}"/>
-    <hyperlink ref="A45" r:id="rId11" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
-    <hyperlink ref="A46" r:id="rId12" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
+    <hyperlink ref="A46" r:id="rId11" xr:uid="{B696A207-AA14-4226-B01D-E4F633E3359E}"/>
+    <hyperlink ref="A47" r:id="rId12" xr:uid="{FC9BFBD5-64DF-4FA5-B956-10395A26F4F7}"/>
     <hyperlink ref="A11" r:id="rId13" xr:uid="{00FD8348-3D5C-4D08-B5A1-80F726E66E33}"/>
     <hyperlink ref="A16" r:id="rId14" display="https://www.digikey.com/product-detail/en/texas-instruments/DRV8872DDAR/296-42661-1-ND/5455926" xr:uid="{6114D03B-D4DA-4FBF-9B1C-C3B7AD098BA9}"/>
     <hyperlink ref="A17" r:id="rId15" display="https://www.digikey.com/product-detail/en/analog-devices-inc/AD7799BRUZ-REEL/AD7799BRUZ-REELCT-ND/4135565" xr:uid="{4B1FE711-B41B-4C95-9AFF-964E590FAEA9}"/>
     <hyperlink ref="A19" r:id="rId16" xr:uid="{C8A12CB4-8BD6-400D-8778-CB90C34529A8}"/>
     <hyperlink ref="A18" r:id="rId17" xr:uid="{DA75B542-D86D-4B8B-A010-0E90403DB631}"/>
-    <hyperlink ref="A14" r:id="rId18" xr:uid="{7F96FA14-D697-422E-905A-991475B71057}"/>
-    <hyperlink ref="A8" r:id="rId19" xr:uid="{9849B45B-0C58-488D-BA9E-5D0A918112A3}"/>
-    <hyperlink ref="A3" r:id="rId20" xr:uid="{0D2ADA9B-1007-4C76-91DB-7B12AE9573EA}"/>
-    <hyperlink ref="A21" r:id="rId21" xr:uid="{1403372D-5EBE-4749-8D7B-B82E7BCD587C}"/>
-    <hyperlink ref="A7" r:id="rId22" xr:uid="{97352714-91EF-4428-A3E4-A04998CB3C31}"/>
-    <hyperlink ref="A20" r:id="rId23" xr:uid="{DB300913-E56B-4B4B-8B6B-45D99AE75B3D}"/>
-    <hyperlink ref="A13" r:id="rId24" xr:uid="{2B494103-7B58-418F-8039-3EE2EE0764D5}"/>
-    <hyperlink ref="A12" r:id="rId25" xr:uid="{FC62576B-0341-4AB6-A60F-37AA4F9AC5C1}"/>
-    <hyperlink ref="A22" r:id="rId26" xr:uid="{143742D2-F4BE-4740-B25E-8DB03D19A806}"/>
-    <hyperlink ref="A10" r:id="rId27" xr:uid="{DCAF167F-0EB9-4809-861C-A6BC048ADE48}"/>
-    <hyperlink ref="A5" r:id="rId28" xr:uid="{E8A4A89C-2D9E-4474-A296-E1633BC9D021}"/>
-    <hyperlink ref="A2" r:id="rId29" xr:uid="{6353ACF5-8899-4C18-9701-ACEEF9533176}"/>
-    <hyperlink ref="A15" r:id="rId30" display="74HC125D" xr:uid="{E676067A-C1FC-4C53-866B-6F5E4C42B0DA}"/>
+    <hyperlink ref="A3" r:id="rId18" xr:uid="{0D2ADA9B-1007-4C76-91DB-7B12AE9573EA}"/>
+    <hyperlink ref="A22" r:id="rId19" xr:uid="{1403372D-5EBE-4749-8D7B-B82E7BCD587C}"/>
+    <hyperlink ref="A7" r:id="rId20" xr:uid="{97352714-91EF-4428-A3E4-A04998CB3C31}"/>
+    <hyperlink ref="A20" r:id="rId21" xr:uid="{DB300913-E56B-4B4B-8B6B-45D99AE75B3D}"/>
+    <hyperlink ref="A13" r:id="rId22" xr:uid="{2B494103-7B58-418F-8039-3EE2EE0764D5}"/>
+    <hyperlink ref="A12" r:id="rId23" xr:uid="{FC62576B-0341-4AB6-A60F-37AA4F9AC5C1}"/>
+    <hyperlink ref="A23" r:id="rId24" xr:uid="{143742D2-F4BE-4740-B25E-8DB03D19A806}"/>
+    <hyperlink ref="A10" r:id="rId25" xr:uid="{DCAF167F-0EB9-4809-861C-A6BC048ADE48}"/>
+    <hyperlink ref="A5" r:id="rId26" xr:uid="{E8A4A89C-2D9E-4474-A296-E1633BC9D021}"/>
+    <hyperlink ref="A2" r:id="rId27" xr:uid="{6353ACF5-8899-4C18-9701-ACEEF9533176}"/>
+    <hyperlink ref="A15" r:id="rId28" display="74HC125D" xr:uid="{E676067A-C1FC-4C53-866B-6F5E4C42B0DA}"/>
+    <hyperlink ref="A8" r:id="rId29" xr:uid="{884D3218-2739-4C0A-BAE2-CD3390E5765E}"/>
+    <hyperlink ref="A14" r:id="rId30" xr:uid="{A9CF932E-1AF1-41C1-8A65-D71C5FB7E107}"/>
+    <hyperlink ref="A21" r:id="rId31" xr:uid="{DD7DCE4D-48AE-496A-8C64-E6F28912AA00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2190,7 +2222,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H44</xm:sqref>
+          <xm:sqref>H45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E5B5708F-AF4E-472B-86D4-E608850ED8C2}">
@@ -2201,7 +2233,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H2:H23</xm:sqref>
+          <xm:sqref>H2:H24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2213,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A2BDBB-E2E5-4A1F-91BC-824E3760DD54}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,29 +2265,29 @@
         <v>2</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -2265,102 +2297,102 @@
     </row>
     <row r="5" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B7" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>121</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,10 +2400,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2379,101 +2411,101 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete PCB version 1
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{870500AA-4E12-4CC9-A815-CB4AFD79983B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B89C069-7417-43FF-BE3E-3D93A437C0B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2246,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added USB port control
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847F24E7-9C50-4620-86EE-FEDA32D943BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C301E02-9152-4A44-9EAC-7D94F543ACB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$25</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="189">
   <si>
     <t>Part Number</t>
   </si>
@@ -560,6 +561,42 @@
   </si>
   <si>
     <t>ABLS-12.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>Pin Group</t>
+  </si>
+  <si>
+    <t>Dataline ESD</t>
+  </si>
+  <si>
+    <t>Power Rail Reverse Polarity</t>
+  </si>
+  <si>
+    <t>Power Rail Over Current</t>
+  </si>
+  <si>
+    <t>Power Rail Switch</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>PMOD Power</t>
+  </si>
+  <si>
+    <t>PMOD IN</t>
+  </si>
+  <si>
+    <t>PMOD Out</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1161,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,4 +2579,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715DDC02-B604-4E22-814C-1C6CA2263E0B}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>